<commit_message>
UI_fix Step1 , Lobby , Step4
</commit_message>
<xml_diff>
--- a/IdensolApp/Assets/Resources/ExcelFiles/MultiLanguage.xlsx
+++ b/IdensolApp/Assets/Resources/ExcelFiles/MultiLanguage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdensolApp\IdensolApp\Assets\Resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811AE47D-95EC-40A9-A676-EB7695BD9062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B54A76-F429-41FE-AA79-D8E341E6CBED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="1440" windowWidth="34365" windowHeight="18150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="2130" windowWidth="34365" windowHeight="18150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="muitiLang" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="809">
   <si>
     <t>id</t>
   </si>
@@ -458,58 +458,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Step1 數位取模</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step1 数位取模</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step1 Digital Scanning</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step2 CAD假牙設計</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step2 CAD假牙设计</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step2 CAD-Prosthetic Design</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step3 CAM假牙排版</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step3 CAM-Prosthetic Planning</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step4 齒雕機加工</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step4 齿雕机加工</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step4  Milling</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step5 燒結烤瓷</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step5 烧结烤瓷</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>看設計步驟</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -586,238 +534,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>創建基底冠訂單</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建基底冠订单</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create a order for copping</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>定義咬合平面</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>定义咬合平面</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Define occlusal plane</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>放置注釋與插入方向</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>放置注释与插入方向</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Optimize directions</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>抓取邊緣線</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>抓取边缘线</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Edit margin line</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>調整代型接口</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整代型接口</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set interfaces</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>設計基底冠</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计基底冠</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Copping design</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>創建解剖冠訂單</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建解剖冠订单</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create a order for crown</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>設計解剖冠</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计解剖冠</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Anatomy design</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>創建嵌體訂單</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建嵌体订单</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create a order for Inlay</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>設計嵌體</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计嵌体</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inlay/Onlay design</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>創建貼面訂單</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建贴面订单</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Create a order for veneer</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>設計貼面</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计贴面</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Veneer design</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>創建基台訂單</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建基台订单</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Defining job details</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>選擇個性化基台</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>选择个性化基台</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set implant type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>掃描桿定位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>扫描杆定位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Detect implant position</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>設計下半部</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计下半部</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generate abutment bottoms</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>放置插入方向</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Define insertion direction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>core型態塑形</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>core型态塑形</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Abutment design</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>設計上半部</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计上半部</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Free-forming</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成基台</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete abutment design</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>氧化鋯</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -835,114 +551,6 @@
   </si>
   <si>
     <t>Glass Cermaic</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>創建氧化鋯項目</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建氧化锆项目</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>載入檔案</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>载入档案</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Import object</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>選擇料盤</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>选择料盘</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Choose materials</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>調整加工位置</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整加工位置</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adjust milling position within material</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>調整支撐棒</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>调整支撑棒</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Move support pin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>點選欲加工策略</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>点选欲加工策略</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Choose milling strategy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>創建玻璃陶瓷項目</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建玻璃陶瓷项目</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>創建Premill項目</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建Premill项目</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>建立植體系統資料庫</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>建立植体系统数据库</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Building implant library</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>點選加工</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>点选加工</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Click to mill</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -2456,11 +2064,6 @@
   </si>
   <si>
     <t>Premill_Build</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Step5 Sintering and
-Crystallization</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -3604,12 +3207,448 @@
     <t>总    公    司</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Digital CAD/CAM systems are no longer the most expensive equipment.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step1&lt;/size&gt; &lt;b&gt;Digital Scanning&lt;/b&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step2&lt;/size&gt; &lt;b&gt;CAD-Prosthetic Design&lt;/b&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step4&lt;/size&gt;  &lt;b&gt;Milling&lt;/b&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step1&lt;/size&gt; 數位取模</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step2&lt;/size&gt; CAD假牙設計</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step3&lt;/size&gt; CAM假牙排版</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step4&lt;/size&gt; 齒雕機加工</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step5&lt;/size&gt; 燒結烤瓷</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step1&lt;/size&gt; 数位取模</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step2&lt;/size&gt; CAD假牙设计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step4&lt;/size&gt; 齿雕机加工</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=36&gt;Step5&lt;/size&gt; 烧结烤瓷</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建基底冠訂單</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step2&lt;/size&gt; 定義咬合平面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 抓取邊緣線</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 放置注釋與插入方向</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 設計基底冠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step5&lt;/size&gt; 調整代型接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建基底冠订单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 放置注释与插入方向</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step2&lt;/size&gt; 定义咬合平面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 抓取边缘线</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step5&lt;/size&gt; 调整代型接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 设计基底冠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step1&lt;/size&gt; Create a order for copping</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step2&lt;/size&gt; Define occlusal plane</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step3&lt;/size&gt; Optimize directions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step4&lt;/size&gt; Edit margin line</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step5&lt;/size&gt; Set interfaces</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step6&lt;/size&gt; Copping design</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建解剖冠訂單</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建嵌體訂單</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建貼面訂單</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建基台訂單</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 設計解剖冠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 設計嵌體</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 設計貼面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step2&lt;/size&gt; 選擇個性化基台</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 掃描桿定位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 設計下半部</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step5&lt;/size&gt; 放置插入方向</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; core型態塑形</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step7&lt;/size&gt; 設計上半部</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step8&lt;/size&gt; 完成基台</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建解剖冠订单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建嵌体订单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建贴面订单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建基台订单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 设计解剖冠</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 设计嵌体</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 设计贴面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step2&lt;/size&gt; 选择个性化基台</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 扫描杆定位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 设计下半部</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; core型态塑形</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step7&lt;/size&gt; 设计上半部</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step1&lt;/size&gt; Create a order for crown</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step1&lt;/size&gt; Create a order for Inlay</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step1&lt;/size&gt; Create a order for veneer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step1&lt;/size&gt; Defining job details</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step6&lt;/size&gt; Anatomy design</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step6&lt;/size&gt; Inlay/Onlay design</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step6&lt;/size&gt; Veneer design</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step2&lt;/size&gt; Set implant type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step3&lt;/size&gt; Detect implant position</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step4&lt;/size&gt; Generate abutment bottoms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step5&lt;/size&gt; Define insertion direction</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step6&lt;/size&gt; Abutment design</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step7&lt;/size&gt; Free-forming</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step8&lt;/size&gt; Complete abutment design</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Premill_Create</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Premill_DefineInsertion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step3&lt;/size&gt; &lt;b&gt;CAM-Prosthetic Planning&lt;/b&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step5&lt;/size&gt; &lt;b&gt;Sintering and Crystallization&lt;/b&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建氧化鋯項目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建玻璃陶瓷項目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 創建Premill項目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step2&lt;/size&gt; 載入檔案</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 選擇料盤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 調整加工位置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step5&lt;/size&gt; 調整支撐棒</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 點選欲加工策略</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 建立植體系統資料庫</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 點選加工</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建氧化锆项目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建玻璃陶瓷项目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step1&lt;/size&gt; 创建Premill项目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step2&lt;/size&gt; 载入档案</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 选择料盘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 调整加工位置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step5&lt;/size&gt; 调整支撑棒</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step6&lt;/size&gt; 点选欲加工策略</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step3&lt;/size&gt; 建立植体系统数据库</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=38&gt;Step4&lt;/size&gt; 点选加工</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step2&lt;/size&gt; Import object</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step3&lt;/size&gt; Choose materials</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step4&lt;/size&gt; Adjust milling position within material</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step5&lt;/size&gt; Move support pin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step6&lt;/size&gt; Choose milling strategy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step3&lt;/size&gt; Building implant library</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;size=30&gt;Step4&lt;/size&gt; Click to mill</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobby_Animation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>動態</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Animate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobby_Model</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>模型</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3674,6 +3713,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3696,7 +3749,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3725,6 +3778,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -4338,10 +4394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D217"/>
+  <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B222" sqref="B222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4377,49 +4433,49 @@
     </row>
     <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>485</v>
+        <v>387</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>482</v>
+        <v>384</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>483</v>
+        <v>385</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>484</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>486</v>
+        <v>388</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>487</v>
+        <v>389</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>487</v>
+        <v>389</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>488</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>491</v>
+        <v>393</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>489</v>
+        <v>391</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>503</v>
+        <v>405</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>490</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>220</v>
+        <v>122</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>62</v>
@@ -4433,7 +4489,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>492</v>
+        <v>394</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
@@ -4447,7 +4503,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>493</v>
+        <v>395</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>68</v>
@@ -4461,7 +4517,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>123</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>70</v>
@@ -4475,7 +4531,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>494</v>
+        <v>396</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>73</v>
@@ -4489,35 +4545,35 @@
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>744</v>
+        <v>645</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>745</v>
+        <v>646</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>746</v>
+        <v>647</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>747</v>
+        <v>648</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>740</v>
+        <v>641</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>741</v>
+        <v>642</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>742</v>
+        <v>643</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>743</v>
+        <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>216</v>
+        <v>118</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>76</v>
@@ -4531,7 +4587,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>217</v>
+        <v>119</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>79</v>
@@ -4545,7 +4601,7 @@
     </row>
     <row r="15" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>218</v>
+        <v>120</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>82</v>
@@ -4559,7 +4615,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>219</v>
+        <v>121</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>85</v>
@@ -4573,7 +4629,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>223</v>
+        <v>125</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>88</v>
@@ -4587,7 +4643,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>222</v>
+        <v>124</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>91</v>
@@ -4601,1279 +4657,1279 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>495</v>
+        <v>397</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>704</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>95</v>
+        <v>709</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>96</v>
+        <v>701</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>496</v>
+        <v>398</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>97</v>
+        <v>705</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>98</v>
+        <v>710</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>99</v>
+        <v>702</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>497</v>
+        <v>399</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>100</v>
+        <v>706</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>101</v>
+        <v>706</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>498</v>
+        <v>400</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>102</v>
+        <v>707</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>103</v>
+        <v>711</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>104</v>
+        <v>703</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>499</v>
+        <v>401</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>105</v>
+        <v>708</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>106</v>
+        <v>712</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>558</v>
+        <v>774</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>500</v>
+        <v>402</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>501</v>
+        <v>403</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>502</v>
+        <v>404</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>511</v>
+        <v>413</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>509</v>
+        <v>411</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>510</v>
+        <v>412</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>508</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>751</v>
+        <v>652</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>749</v>
+        <v>650</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>749</v>
+        <v>650</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>750</v>
+        <v>651</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>767</v>
+        <v>668</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>752</v>
+        <v>653</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>757</v>
+        <v>658</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>762</v>
+        <v>663</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>768</v>
+        <v>669</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>753</v>
+        <v>654</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>758</v>
+        <v>659</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>763</v>
+        <v>664</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>770</v>
+        <v>671</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>754</v>
+        <v>655</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>759</v>
+        <v>660</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>764</v>
+        <v>665</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>771</v>
+        <v>672</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>755</v>
+        <v>656</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>760</v>
+        <v>661</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>765</v>
+        <v>666</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>772</v>
+        <v>673</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>756</v>
+        <v>657</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>761</v>
+        <v>662</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>766</v>
+        <v>667</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>779</v>
+        <v>680</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>773</v>
+        <v>674</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>774</v>
+        <v>675</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>777</v>
+        <v>678</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>780</v>
+        <v>681</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>775</v>
+        <v>676</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>776</v>
+        <v>677</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>778</v>
+        <v>679</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>507</v>
+        <v>409</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>504</v>
+        <v>406</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>505</v>
+        <v>407</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>506</v>
+        <v>408</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>512</v>
+        <v>414</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>769</v>
+        <v>670</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>513</v>
+        <v>415</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>514</v>
+        <v>416</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>515</v>
+        <v>417</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>516</v>
+        <v>418</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>126</v>
+        <v>713</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>127</v>
+        <v>719</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>128</v>
+        <v>725</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>517</v>
+        <v>419</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>129</v>
+        <v>714</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>130</v>
+        <v>721</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>131</v>
+        <v>726</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>518</v>
+        <v>420</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>132</v>
+        <v>716</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>133</v>
+        <v>720</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>134</v>
+        <v>727</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>519</v>
+        <v>421</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>135</v>
+        <v>715</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>136</v>
+        <v>722</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>137</v>
+        <v>728</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>138</v>
+        <v>718</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>139</v>
+        <v>723</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>140</v>
+        <v>729</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>521</v>
+        <v>423</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>141</v>
+        <v>717</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>142</v>
+        <v>724</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>143</v>
+        <v>730</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>522</v>
+        <v>424</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>144</v>
+        <v>731</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>145</v>
+        <v>745</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>146</v>
+        <v>757</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>523</v>
+        <v>425</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>129</v>
+        <v>714</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>130</v>
+        <v>721</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>131</v>
+        <v>726</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>524</v>
+        <v>426</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>132</v>
+        <v>716</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>133</v>
+        <v>720</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>134</v>
+        <v>727</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>525</v>
+        <v>427</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>135</v>
+        <v>715</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>136</v>
+        <v>722</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>137</v>
+        <v>728</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>526</v>
+        <v>428</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>138</v>
+        <v>718</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>139</v>
+        <v>723</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>140</v>
+        <v>729</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>527</v>
+        <v>429</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>147</v>
+        <v>735</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>148</v>
+        <v>749</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>149</v>
+        <v>761</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>528</v>
+        <v>430</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>150</v>
+        <v>732</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>151</v>
+        <v>746</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>152</v>
+        <v>758</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>529</v>
+        <v>431</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>129</v>
+        <v>714</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>130</v>
+        <v>721</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>131</v>
+        <v>726</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>530</v>
+        <v>432</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>132</v>
+        <v>716</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>133</v>
+        <v>720</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>134</v>
+        <v>727</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>531</v>
+        <v>433</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>135</v>
+        <v>715</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>136</v>
+        <v>722</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>137</v>
+        <v>728</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>532</v>
+        <v>434</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>138</v>
+        <v>718</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>139</v>
+        <v>723</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>140</v>
+        <v>729</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>533</v>
+        <v>435</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>153</v>
+        <v>736</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>154</v>
+        <v>750</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>155</v>
+        <v>762</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>535</v>
+        <v>437</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>156</v>
+        <v>733</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>157</v>
+        <v>747</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>158</v>
+        <v>759</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>536</v>
+        <v>438</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>129</v>
+        <v>714</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>130</v>
+        <v>721</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>131</v>
+        <v>726</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>537</v>
+        <v>439</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>132</v>
+        <v>716</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>133</v>
+        <v>720</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>134</v>
+        <v>727</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>538</v>
+        <v>440</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>135</v>
+        <v>715</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>136</v>
+        <v>722</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>137</v>
+        <v>728</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>539</v>
+        <v>441</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>138</v>
+        <v>718</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>139</v>
+        <v>723</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>140</v>
+        <v>729</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>534</v>
+        <v>436</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>159</v>
+        <v>737</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>160</v>
+        <v>751</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>161</v>
+        <v>763</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>540</v>
+        <v>771</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>162</v>
+        <v>734</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>163</v>
+        <v>748</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>164</v>
+        <v>760</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>541</v>
+        <v>443</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>165</v>
+        <v>738</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>166</v>
+        <v>752</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>167</v>
+        <v>764</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>542</v>
+        <v>444</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>168</v>
+        <v>739</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>169</v>
+        <v>753</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>170</v>
+        <v>765</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>543</v>
+        <v>445</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>171</v>
+        <v>740</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>172</v>
+        <v>754</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>173</v>
+        <v>766</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>540</v>
+        <v>772</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>174</v>
+        <v>741</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>174</v>
+        <v>741</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>175</v>
+        <v>767</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>544</v>
+        <v>446</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>176</v>
+        <v>742</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>177</v>
+        <v>755</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>178</v>
+        <v>768</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>545</v>
+        <v>447</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>179</v>
+        <v>743</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>180</v>
+        <v>756</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>181</v>
+        <v>769</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>546</v>
+        <v>448</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>182</v>
+        <v>744</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>182</v>
+        <v>744</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>183</v>
+        <v>770</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>547</v>
+        <v>449</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>185</v>
+        <v>114</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>559</v>
+        <v>460</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>187</v>
+        <v>116</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>548</v>
+        <v>450</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>790</v>
+        <v>691</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>785</v>
+        <v>686</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>793</v>
+        <v>694</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>796</v>
+        <v>697</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>791</v>
+        <v>692</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>787</v>
+        <v>688</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>786</v>
+        <v>687</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>795</v>
+        <v>696</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>792</v>
+        <v>693</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>789</v>
+        <v>690</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>788</v>
+        <v>689</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>794</v>
+        <v>695</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>784</v>
+        <v>685</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>781</v>
+        <v>682</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>782</v>
+        <v>683</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>783</v>
+        <v>684</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>549</v>
+        <v>451</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>189</v>
+        <v>775</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>190</v>
+        <v>785</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>164</v>
+        <v>760</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>550</v>
+        <v>452</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>191</v>
+        <v>778</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>192</v>
+        <v>788</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>193</v>
+        <v>795</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>554</v>
+        <v>456</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>194</v>
+        <v>779</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>195</v>
+        <v>789</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>196</v>
+        <v>796</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>552</v>
+        <v>454</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>197</v>
+        <v>780</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>198</v>
+        <v>790</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>199</v>
+        <v>797</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>553</v>
+        <v>455</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>200</v>
+        <v>781</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>201</v>
+        <v>791</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>202</v>
+        <v>798</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>551</v>
+        <v>453</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>203</v>
+        <v>782</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>204</v>
+        <v>792</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>205</v>
+        <v>799</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>560</v>
+        <v>461</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>206</v>
+        <v>776</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>207</v>
+        <v>786</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>164</v>
+        <v>760</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>561</v>
+        <v>462</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>191</v>
+        <v>778</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>192</v>
+        <v>788</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>193</v>
+        <v>795</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>562</v>
+        <v>463</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>194</v>
+        <v>779</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>195</v>
+        <v>789</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>196</v>
+        <v>796</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>563</v>
+        <v>464</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>197</v>
+        <v>780</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>198</v>
+        <v>790</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>199</v>
+        <v>797</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>564</v>
+        <v>465</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>200</v>
+        <v>781</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>201</v>
+        <v>791</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>202</v>
+        <v>798</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>565</v>
+        <v>466</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>203</v>
+        <v>782</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>204</v>
+        <v>792</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>205</v>
+        <v>799</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>540</v>
+        <v>442</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>208</v>
+        <v>777</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>209</v>
+        <v>787</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>164</v>
+        <v>760</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>555</v>
+        <v>457</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>191</v>
+        <v>778</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>192</v>
+        <v>788</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>193</v>
+        <v>795</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>557</v>
+        <v>459</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>210</v>
+        <v>783</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>211</v>
+        <v>793</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>212</v>
+        <v>800</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>556</v>
+        <v>458</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>213</v>
+        <v>784</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>214</v>
+        <v>794</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>215</v>
+        <v>801</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>566</v>
+        <v>467</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>230</v>
+        <v>132</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>231</v>
+        <v>133</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>232</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>567</v>
+        <v>468</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>233</v>
+        <v>135</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>234</v>
+        <v>136</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>235</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>568</v>
+        <v>469</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>236</v>
+        <v>138</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>237</v>
+        <v>139</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>238</v>
+        <v>140</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>569</v>
+        <v>470</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>239</v>
+        <v>141</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>240</v>
+        <v>142</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>241</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>570</v>
+        <v>471</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>242</v>
+        <v>144</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>243</v>
+        <v>145</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>244</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>571</v>
+        <v>472</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>245</v>
+        <v>147</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>246</v>
+        <v>148</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>247</v>
+        <v>149</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>638</v>
+        <v>539</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>248</v>
+        <v>150</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>249</v>
+        <v>151</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>250</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>639</v>
+        <v>540</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>224</v>
+        <v>126</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>226</v>
+        <v>128</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>228</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>640</v>
+        <v>541</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>225</v>
+        <v>127</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>227</v>
+        <v>129</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>229</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
       <c r="B106" s="3" t="s">
-        <v>261</v>
+        <v>163</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>262</v>
+        <v>164</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>263</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
       <c r="B107" s="3" t="s">
-        <v>251</v>
+        <v>153</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>255</v>
+        <v>157</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>258</v>
+        <v>160</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
       <c r="B108" s="3" t="s">
-        <v>252</v>
+        <v>154</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>256</v>
+        <v>158</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>259</v>
+        <v>161</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
       <c r="B109" s="3" t="s">
-        <v>253</v>
+        <v>155</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>260</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>671</v>
+        <v>572</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>254</v>
+        <v>156</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>254</v>
+        <v>156</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>93</v>
@@ -5881,111 +5937,111 @@
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>653</v>
+        <v>554</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>641</v>
+        <v>542</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>642</v>
+        <v>543</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>643</v>
+        <v>544</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>654</v>
+        <v>555</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>644</v>
+        <v>545</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>645</v>
+        <v>546</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>646</v>
+        <v>547</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>655</v>
+        <v>556</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>647</v>
+        <v>548</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>648</v>
+        <v>549</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>649</v>
+        <v>550</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>656</v>
+        <v>557</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>650</v>
+        <v>551</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>651</v>
+        <v>552</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>652</v>
+        <v>553</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>657</v>
+        <v>558</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>264</v>
+        <v>166</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>265</v>
+        <v>167</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>266</v>
+        <v>168</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>664</v>
+        <v>565</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>661</v>
+        <v>562</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>662</v>
+        <v>563</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>663</v>
+        <v>564</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>665</v>
+        <v>566</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>267</v>
+        <v>169</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>267</v>
+        <v>169</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>268</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>666</v>
+        <v>567</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>269</v>
+        <v>171</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>270</v>
+        <v>172</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>64</v>
@@ -5993,51 +6049,51 @@
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>667</v>
+        <v>568</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>271</v>
+        <v>173</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>272</v>
+        <v>174</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>273</v>
+        <v>175</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>670</v>
+        <v>571</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>668</v>
+        <v>569</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>668</v>
+        <v>569</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>669</v>
+        <v>570</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
       <c r="B121" s="3" t="s">
-        <v>274</v>
+        <v>176</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>275</v>
+        <v>177</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>276</v>
+        <v>178</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="2" t="s">
-        <v>254</v>
+        <v>156</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>680</v>
+        <v>581</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>93</v>
@@ -6045,116 +6101,116 @@
     </row>
     <row r="123" spans="1:4" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>673</v>
+        <v>574</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>672</v>
+        <v>573</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>672</v>
+        <v>573</v>
       </c>
       <c r="D123" s="3"/>
     </row>
     <row r="124" spans="1:4" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>686</v>
+        <v>587</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>674</v>
+        <v>575</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>677</v>
+        <v>578</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>682</v>
+        <v>583</v>
       </c>
     </row>
     <row r="125" spans="1:4" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>687</v>
+        <v>588</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>688</v>
+        <v>589</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>678</v>
+        <v>579</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>683</v>
+        <v>584</v>
       </c>
     </row>
     <row r="126" spans="1:4" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>689</v>
+        <v>590</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>675</v>
+        <v>576</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>679</v>
+        <v>580</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>684</v>
+        <v>585</v>
       </c>
     </row>
     <row r="127" spans="1:4" s="8" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>690</v>
+        <v>591</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>676</v>
+        <v>577</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>681</v>
+        <v>582</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>685</v>
+        <v>586</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>658</v>
+        <v>559</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>277</v>
+        <v>179</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>278</v>
+        <v>180</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>279</v>
+        <v>181</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
-        <v>280</v>
+        <v>182</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>281</v>
+        <v>183</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>282</v>
+        <v>184</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
-        <v>283</v>
+        <v>185</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>284</v>
+        <v>186</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>285</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>691</v>
+        <v>592</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>286</v>
+        <v>188</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>89</v>
@@ -6165,1167 +6221,1197 @@
     </row>
     <row r="132" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>706</v>
+        <v>607</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>287</v>
+        <v>189</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>288</v>
+        <v>190</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>289</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>659</v>
+        <v>560</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>290</v>
+        <v>192</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>291</v>
+        <v>193</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>292</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>601</v>
+        <v>502</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>293</v>
+        <v>195</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>293</v>
+        <v>195</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>294</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>660</v>
+        <v>561</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>295</v>
+        <v>197</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>296</v>
+        <v>198</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>297</v>
+        <v>199</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>692</v>
+        <v>593</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>298</v>
+        <v>200</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>299</v>
+        <v>201</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>300</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>693</v>
+        <v>594</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>301</v>
+        <v>203</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>302</v>
+        <v>204</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>303</v>
+        <v>205</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>694</v>
+        <v>595</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>304</v>
+        <v>206</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>305</v>
+        <v>207</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>306</v>
+        <v>208</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>695</v>
+        <v>596</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>307</v>
+        <v>209</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>308</v>
+        <v>210</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>309</v>
+        <v>211</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>697</v>
+        <v>598</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>310</v>
+        <v>212</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>311</v>
+        <v>213</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>696</v>
+        <v>597</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>698</v>
+        <v>599</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>312</v>
+        <v>214</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>313</v>
+        <v>215</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>314</v>
+        <v>216</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>699</v>
+        <v>600</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>315</v>
+        <v>217</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>316</v>
+        <v>218</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>317</v>
+        <v>219</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>700</v>
+        <v>601</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>318</v>
+        <v>220</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>319</v>
+        <v>221</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>320</v>
+        <v>222</v>
       </c>
     </row>
     <row r="144" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
-        <v>701</v>
+        <v>602</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>476</v>
+        <v>378</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>477</v>
+        <v>379</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>480</v>
+        <v>382</v>
       </c>
     </row>
     <row r="145" spans="1:4" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
-        <v>702</v>
+        <v>603</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>479</v>
+        <v>381</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>478</v>
+        <v>380</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>321</v>
+        <v>223</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>703</v>
+        <v>604</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>322</v>
+        <v>224</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>323</v>
+        <v>225</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>324</v>
+        <v>226</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>704</v>
+        <v>605</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>325</v>
+        <v>227</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>326</v>
+        <v>228</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>327</v>
+        <v>229</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>705</v>
+        <v>606</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>328</v>
+        <v>230</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>329</v>
+        <v>231</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>330</v>
+        <v>232</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>578</v>
+        <v>479</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>572</v>
+        <v>473</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>574</v>
+        <v>475</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>576</v>
+        <v>477</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>579</v>
+        <v>480</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>573</v>
+        <v>474</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>575</v>
+        <v>476</v>
       </c>
       <c r="D150" s="7" t="s">
-        <v>577</v>
+        <v>478</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>597</v>
+        <v>498</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>331</v>
+        <v>233</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>332</v>
+        <v>234</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>748</v>
+        <v>649</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>598</v>
+        <v>499</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>333</v>
+        <v>235</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>334</v>
+        <v>236</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>335</v>
+        <v>237</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
-        <v>596</v>
+        <v>497</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>336</v>
+        <v>238</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>337</v>
+        <v>239</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>338</v>
+        <v>240</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
-        <v>599</v>
+        <v>500</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>339</v>
+        <v>241</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>340</v>
+        <v>242</v>
       </c>
       <c r="D154" s="7" t="s">
-        <v>341</v>
+        <v>243</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
-        <v>600</v>
+        <v>501</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>342</v>
+        <v>244</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>343</v>
+        <v>245</v>
       </c>
       <c r="D155" s="7" t="s">
-        <v>344</v>
+        <v>246</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>595</v>
+        <v>496</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>589</v>
+        <v>490</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>588</v>
+        <v>489</v>
       </c>
       <c r="D156" s="7" t="s">
-        <v>587</v>
+        <v>488</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>594</v>
+        <v>495</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>580</v>
+        <v>481</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>583</v>
+        <v>484</v>
       </c>
       <c r="D157" s="7" t="s">
-        <v>585</v>
+        <v>486</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
-        <v>593</v>
+        <v>494</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>581</v>
+        <v>482</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>590</v>
+        <v>491</v>
       </c>
       <c r="D158" s="7" t="s">
-        <v>586</v>
+        <v>487</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>592</v>
+        <v>493</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>582</v>
+        <v>483</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>584</v>
+        <v>485</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>591</v>
+        <v>492</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
-        <v>607</v>
+        <v>508</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>604</v>
+        <v>505</v>
       </c>
       <c r="C160" s="7" t="s">
-        <v>605</v>
+        <v>506</v>
       </c>
       <c r="D160" s="7" t="s">
-        <v>606</v>
+        <v>507</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
-        <v>631</v>
+        <v>532</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>618</v>
+        <v>519</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>619</v>
+        <v>520</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>620</v>
+        <v>521</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
-        <v>632</v>
+        <v>533</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>621</v>
+        <v>522</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>622</v>
+        <v>523</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>623</v>
+        <v>524</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
-        <v>633</v>
+        <v>534</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>624</v>
+        <v>525</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>629</v>
+        <v>530</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>630</v>
+        <v>531</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>602</v>
+        <v>503</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>345</v>
+        <v>247</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>346</v>
+        <v>248</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>347</v>
+        <v>249</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>608</v>
+        <v>509</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>348</v>
+        <v>250</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>349</v>
+        <v>251</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>350</v>
+        <v>252</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>610</v>
+        <v>511</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>611</v>
+        <v>512</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>612</v>
+        <v>513</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>351</v>
+        <v>253</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>609</v>
+        <v>510</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>352</v>
+        <v>254</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>353</v>
+        <v>255</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>354</v>
+        <v>256</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>603</v>
+        <v>504</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>355</v>
+        <v>257</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>356</v>
+        <v>258</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>357</v>
+        <v>259</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>613</v>
+        <v>514</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>358</v>
+        <v>260</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>359</v>
+        <v>261</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>360</v>
+        <v>262</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>614</v>
+        <v>515</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>361</v>
+        <v>263</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>362</v>
+        <v>264</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>363</v>
+        <v>265</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3"/>
       <c r="B171" s="3" t="s">
-        <v>352</v>
+        <v>254</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>353</v>
+        <v>255</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>354</v>
+        <v>256</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>615</v>
+        <v>516</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>625</v>
+        <v>526</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>626</v>
+        <v>527</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>364</v>
+        <v>266</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>616</v>
+        <v>517</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>628</v>
+        <v>529</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>627</v>
+        <v>528</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>365</v>
+        <v>267</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>617</v>
+        <v>518</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>366</v>
+        <v>268</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>367</v>
+        <v>269</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>368</v>
+        <v>270</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
       <c r="B175" s="3" t="s">
-        <v>352</v>
+        <v>254</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>353</v>
+        <v>255</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>354</v>
+        <v>256</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>721</v>
+        <v>622</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>369</v>
+        <v>271</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>370</v>
+        <v>272</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>371</v>
+        <v>273</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3"/>
       <c r="B177" s="7" t="s">
-        <v>372</v>
+        <v>274</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>373</v>
+        <v>275</v>
       </c>
       <c r="D177" s="7" t="s">
-        <v>374</v>
+        <v>276</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>722</v>
+        <v>623</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>375</v>
+        <v>277</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>376</v>
+        <v>278</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>377</v>
+        <v>279</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="3"/>
       <c r="B179" s="3" t="s">
-        <v>378</v>
+        <v>280</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>379</v>
+        <v>281</v>
       </c>
       <c r="D179" s="7" t="s">
-        <v>380</v>
+        <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>723</v>
+        <v>624</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>381</v>
+        <v>283</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>382</v>
+        <v>284</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>383</v>
+        <v>285</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="3"/>
       <c r="B181" s="3" t="s">
-        <v>384</v>
+        <v>286</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>385</v>
+        <v>287</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>386</v>
+        <v>288</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>724</v>
+        <v>625</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>387</v>
+        <v>289</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>388</v>
+        <v>290</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>389</v>
+        <v>291</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="3"/>
       <c r="B183" s="3" t="s">
-        <v>390</v>
+        <v>292</v>
       </c>
       <c r="C183" s="7" t="s">
-        <v>391</v>
+        <v>293</v>
       </c>
       <c r="D183" s="7" t="s">
-        <v>392</v>
+        <v>294</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>725</v>
+        <v>626</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>393</v>
+        <v>295</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>394</v>
+        <v>296</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>395</v>
+        <v>297</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="3"/>
       <c r="B185" s="7" t="s">
-        <v>396</v>
+        <v>298</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>397</v>
+        <v>299</v>
       </c>
       <c r="D185" s="7" t="s">
-        <v>481</v>
+        <v>383</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>726</v>
+        <v>627</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>398</v>
+        <v>300</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>399</v>
+        <v>301</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>400</v>
+        <v>302</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="3"/>
       <c r="B187" s="3" t="s">
-        <v>401</v>
+        <v>303</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>402</v>
+        <v>304</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>727</v>
+        <v>628</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>404</v>
+        <v>306</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>405</v>
+        <v>307</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>406</v>
+        <v>308</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="3"/>
       <c r="B189" s="3" t="s">
-        <v>384</v>
+        <v>286</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>385</v>
+        <v>287</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>386</v>
+        <v>288</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>728</v>
+        <v>629</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>407</v>
+        <v>309</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>408</v>
+        <v>310</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>409</v>
+        <v>311</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="3"/>
       <c r="B191" s="7" t="s">
-        <v>410</v>
+        <v>312</v>
       </c>
       <c r="C191" s="7" t="s">
-        <v>411</v>
+        <v>313</v>
       </c>
       <c r="D191" s="7" t="s">
-        <v>637</v>
+        <v>538</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>729</v>
+        <v>630</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>412</v>
+        <v>314</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>413</v>
+        <v>315</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>414</v>
+        <v>316</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3"/>
       <c r="B193" s="7" t="s">
-        <v>415</v>
+        <v>317</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>416</v>
+        <v>318</v>
       </c>
       <c r="D193" s="7" t="s">
-        <v>636</v>
+        <v>537</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>730</v>
+        <v>631</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>417</v>
+        <v>319</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>418</v>
+        <v>320</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>419</v>
+        <v>321</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>
       <c r="B195" s="3" t="s">
-        <v>420</v>
+        <v>322</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>421</v>
+        <v>323</v>
       </c>
       <c r="D195" s="7" t="s">
-        <v>422</v>
+        <v>324</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>731</v>
+        <v>632</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>423</v>
+        <v>325</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>424</v>
+        <v>326</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>425</v>
+        <v>327</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3"/>
       <c r="B197" s="7" t="s">
-        <v>426</v>
+        <v>328</v>
       </c>
       <c r="C197" s="7" t="s">
-        <v>427</v>
+        <v>329</v>
       </c>
       <c r="D197" s="7" t="s">
-        <v>634</v>
+        <v>535</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>732</v>
+        <v>633</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>428</v>
+        <v>330</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>429</v>
+        <v>331</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>430</v>
+        <v>332</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3"/>
       <c r="B199" s="7" t="s">
-        <v>431</v>
+        <v>333</v>
       </c>
       <c r="C199" s="7" t="s">
-        <v>432</v>
+        <v>334</v>
       </c>
       <c r="D199" s="7" t="s">
-        <v>635</v>
+        <v>536</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>733</v>
+        <v>634</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>433</v>
+        <v>335</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>434</v>
+        <v>336</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>435</v>
+        <v>337</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="3"/>
       <c r="B201" s="7" t="s">
-        <v>436</v>
+        <v>338</v>
       </c>
       <c r="C201" s="7" t="s">
-        <v>437</v>
+        <v>339</v>
       </c>
       <c r="D201" s="7" t="s">
-        <v>438</v>
+        <v>340</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="3"/>
       <c r="B202" s="7" t="s">
-        <v>439</v>
+        <v>341</v>
       </c>
       <c r="C202" s="7" t="s">
-        <v>440</v>
+        <v>342</v>
       </c>
       <c r="D202" s="7" t="s">
-        <v>441</v>
+        <v>343</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="3"/>
       <c r="B203" s="7" t="s">
-        <v>442</v>
+        <v>344</v>
       </c>
       <c r="C203" s="7" t="s">
-        <v>443</v>
+        <v>345</v>
       </c>
       <c r="D203" s="7" t="s">
-        <v>444</v>
+        <v>346</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>708</v>
+        <v>609</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>797</v>
+        <v>698</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>798</v>
+        <v>699</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>707</v>
+        <v>608</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>709</v>
+        <v>610</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>445</v>
+        <v>347</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>446</v>
+        <v>348</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>447</v>
+        <v>349</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>710</v>
+        <v>611</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>448</v>
+        <v>350</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>449</v>
+        <v>351</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>450</v>
+        <v>352</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>711</v>
+        <v>612</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>451</v>
+        <v>353</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>451</v>
+        <v>353</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>452</v>
+        <v>354</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>712</v>
+        <v>613</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>453</v>
+        <v>355</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>454</v>
+        <v>356</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>455</v>
+        <v>357</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>713</v>
+        <v>614</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>456</v>
+        <v>358</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>457</v>
+        <v>359</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>458</v>
+        <v>360</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>714</v>
+        <v>615</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>459</v>
+        <v>361</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>460</v>
+        <v>362</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>461</v>
+        <v>363</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>715</v>
+        <v>616</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>462</v>
+        <v>364</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>464</v>
+        <v>366</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>716</v>
+        <v>617</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>465</v>
+        <v>367</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>466</v>
+        <v>368</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>467</v>
+        <v>369</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>719</v>
+        <v>620</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>468</v>
+        <v>370</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="D213" s="3"/>
+        <v>371</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="214" spans="1:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>720</v>
+        <v>621</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>470</v>
+        <v>372</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>471</v>
+        <v>373</v>
       </c>
       <c r="D214" s="7" t="s">
-        <v>472</v>
+        <v>374</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>717</v>
+        <v>618</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>473</v>
+        <v>375</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>474</v>
+        <v>376</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>475</v>
+        <v>377</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>718</v>
+        <v>619</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>734</v>
+        <v>635</v>
       </c>
       <c r="C216" s="7" t="s">
-        <v>736</v>
+        <v>637</v>
       </c>
       <c r="D216" s="7" t="s">
-        <v>738</v>
+        <v>639</v>
       </c>
     </row>
     <row r="217" spans="1:4" s="8" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="9" t="s">
-        <v>735</v>
+        <v>636</v>
       </c>
       <c r="C217" s="10" t="s">
-        <v>737</v>
+        <v>638</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>739</v>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="B218" s="13" t="s">
+        <v>803</v>
+      </c>
+      <c r="C218" s="14" t="s">
+        <v>804</v>
+      </c>
+      <c r="D218" s="12" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="B219" s="13" t="s">
+        <v>807</v>
+      </c>
+      <c r="C219" s="13" t="s">
+        <v>807</v>
+      </c>
+      <c r="D219" s="12" t="s">
+        <v>808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>